<commit_message>
obat dan produsen terbanyak
</commit_message>
<xml_diff>
--- a/excel/format/data.xlsx
+++ b/excel/format/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dashboardapotik\excel\format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9715086C-3958-4649-932D-61DAFE11A597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751AF534-CC1F-4ACC-B4C4-E23BFF1E89FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D30C9278-207D-415C-9E7B-8C0ACF7B1875}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{D30C9278-207D-415C-9E7B-8C0ACF7B1875}"/>
   </bookViews>
   <sheets>
     <sheet name="kategori" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>nama</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>jenis bayar</t>
+  </si>
+  <si>
+    <t>time</t>
   </si>
 </sst>
 </file>
@@ -467,7 +470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5959E06-8FA6-41AE-B972-6DDCB35664C8}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -618,10 +621,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECE7FFA-EC79-4AC4-81F2-57E9B2BDEA11}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,12 +638,15 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>